<commit_message>
refactor: remove holder name normalization for consistent raw data use
</commit_message>
<xml_diff>
--- a/akses_cleaned102.xlsx
+++ b/akses_cleaned102.xlsx
@@ -562,7 +562,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dea Rahmawati</t>
+          <t>dea rahmawati</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -608,7 +608,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dea Rahmawati</t>
+          <t>dea rahmawati</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -654,7 +654,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dea Rahmawati</t>
+          <t>dea rahmawati</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -700,7 +700,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Dea Rahmawati</t>
+          <t>dea rahmawati</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -746,7 +746,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Housekeeping</t>
+          <t>HOUSEKEEPING</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -804,7 +804,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ronald Mulyo</t>
+          <t>ronald mulyo</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -850,7 +850,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ronald Mulyo</t>
+          <t>ronald mulyo</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -896,7 +896,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Ronald Mulyo</t>
+          <t>ronald mulyo</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -942,7 +942,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Ronald Mulyo</t>
+          <t>ronald mulyo</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Ronald Mulyo</t>
+          <t>ronald mulyo</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Ronald Mulyo</t>
+          <t>ronald mulyo</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Ronald Mulyo</t>
+          <t>ronald mulyo</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Ronald Mulyo</t>
+          <t>ronald mulyo</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Housekeeping</t>
+          <t>HOUSEKEEPING</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Housekeeping</t>
+          <t>HOUSEKEEPING</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Fian Agung Triantoro</t>
+          <t>fian agung triantoro</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>

</xml_diff>